<commit_message>
completed updates and BOM
</commit_message>
<xml_diff>
--- a/BOM/Eco_display.xlsx
+++ b/BOM/Eco_display.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\kicad6\KICAD 6.0.0\contractual_projects\ECO_BODA\Display_Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{441FA23D-2DBD-467B-A24D-A5BD19276A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{10E0CF09-39F4-4072-B0B9-1DBF512CE8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Eco_display" sheetId="1" r:id="rId1"/>
@@ -117,15 +117,6 @@
     <t>220R</t>
   </si>
   <si>
-    <t>SW1, SW2, SW3</t>
-  </si>
-  <si>
-    <t>SW_Push</t>
-  </si>
-  <si>
-    <t>MACHADA_footprints:sw_memebrane_btn_SK5AM00300</t>
-  </si>
-  <si>
     <t>U4, U6</t>
   </si>
   <si>
@@ -174,14 +165,23 @@
     <t>0402WGF2200TCE</t>
   </si>
   <si>
-    <t>SK5AM00300</t>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>ZX-PZ2.54-2-4PWZ</t>
+  </si>
+  <si>
+    <t>Connector_PinHeader_2.54mm:PinHeader_1x04_P2.54mm_Horizontal</t>
+  </si>
+  <si>
+    <t>Conn_01x04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +312,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -620,7 +628,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -663,15 +671,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -705,6 +715,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1024,11 +1035,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1050,10 +1061,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>0</v>
@@ -1070,10 +1081,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F2">
         <v>2</v>
@@ -1090,10 +1101,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1113,7 +1124,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -1133,7 +1144,7 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1153,7 +1164,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1170,10 +1181,10 @@
         <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1190,10 +1201,10 @@
         <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1210,10 +1221,10 @@
         <v>23</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F9">
         <v>2</v>
@@ -1230,10 +1241,10 @@
         <v>23</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -1250,10 +1261,10 @@
         <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1261,19 +1272,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
+        <v>49</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F12">
         <v>3</v>
@@ -1281,19 +1292,19 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F13">
         <v>2</v>
@@ -1301,19 +1312,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1321,7 +1332,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
coplete addition of BOM and placement guide pdf files
</commit_message>
<xml_diff>
--- a/BOM/Eco_display.xlsx
+++ b/BOM/Eco_display.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\kicad6\KICAD 6.0.0\contractual_projects\ECO_BODA\Display_Board\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{42999027-1819-446F-86E6-862A8EE988DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE556FCA-1AC4-472B-AD16-98B71904EEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
   </bookViews>
   <sheets>
     <sheet name="Eco_display" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="71" uniqueCount="50">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="91" uniqueCount="62">
   <si>
     <t>Qty</t>
   </si>
@@ -39,6 +39,21 @@
     <t>Footprint</t>
   </si>
   <si>
+    <t>MPN</t>
+  </si>
+  <si>
+    <t>BZ1</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>Buzzer_Beeper:MagneticBuzzer_ProSignal_ABT-410-RC</t>
+  </si>
+  <si>
+    <t>GMC12038YA-16R2048</t>
+  </si>
+  <si>
     <t>C30, C31</t>
   </si>
   <si>
@@ -99,6 +114,24 @@
     <t>Connector_PinHeader_2.54mm:PinHeader_1x04_P2.54mm_Horizontal</t>
   </si>
   <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Inductor_SMD:L_0402_1005Metric</t>
+  </si>
+  <si>
+    <t>BLM15HD182SN1D</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>BSN20</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -108,6 +141,18 @@
     <t>Resistor_SMD:R_0402_1005Metric</t>
   </si>
   <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>Resistor_SMD:R_0603_1608Metric</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
     <t>R31, R32</t>
   </si>
   <si>
@@ -126,15 +171,6 @@
     <t>220R</t>
   </si>
   <si>
-    <t>U4, U6</t>
-  </si>
-  <si>
-    <t>TBU-CA065-200-WH</t>
-  </si>
-  <si>
-    <t>MACHADA_footprints:TBU-CA065-200-WH</t>
-  </si>
-  <si>
     <t>U19</t>
   </si>
   <si>
@@ -144,9 +180,6 @@
     <t>Package_SO:MSOP-8_3x3mm_P0.65mm</t>
   </si>
   <si>
-    <t>MPN</t>
-  </si>
-  <si>
     <t>Vendor</t>
   </si>
   <si>
@@ -159,9 +192,15 @@
     <t>HC-5557-2*4AW</t>
   </si>
   <si>
+    <t>ZX-PZ2.54-2-4PWZ</t>
+  </si>
+  <si>
     <t>RC0402FR-0710KL</t>
   </si>
   <si>
+    <t>RC0402FR-7W1KL</t>
+  </si>
+  <si>
     <t>RC0402FR-07100KL</t>
   </si>
   <si>
@@ -169,9 +208,6 @@
   </si>
   <si>
     <t>0402WGF2200TCE</t>
-  </si>
-  <si>
-    <t>ZX-PZ2.54-2-4PWZ</t>
   </si>
   <si>
     <t>LCSC</t>
@@ -181,7 +217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,6 +348,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -666,10 +708,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1025,301 +1067,382 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="27.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" customWidth="1"/>
+    <col min="2" max="3" width="28.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>49</v>
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>49</v>
+      <c r="D4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
+        <v>16</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6">
         <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
-      </c>
-      <c r="E7">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7">
         <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E8">
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8">
         <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E9">
+        <v>28</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9">
         <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10">
         <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="F11" t="s">
-        <v>49</v>
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12">
         <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>49</v>
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="D15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
       </c>
-      <c r="E14">
+      <c r="D16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17">
         <v>1</v>
       </c>
-      <c r="F14" t="s">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
         <v>49</v>
       </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>